<commit_message>
se actualiza para correr Perfiles
</commit_message>
<xml_diff>
--- a/src/test/resources/Datadriven/Express300.xlsx
+++ b/src/test/resources/Datadriven/Express300.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="30" windowWidth="20115" windowHeight="7485" activeTab="1"/>
+    <workbookView xWindow="240" yWindow="30" windowWidth="20115" windowHeight="7485"/>
   </bookViews>
   <sheets>
     <sheet name="ProyectoSolucion" sheetId="4" r:id="rId1"/>
@@ -419,7 +419,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -427,13 +427,44 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="3" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="3" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -448,10 +479,15 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="49" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="49" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="49" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="49" fontId="0" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -771,8 +807,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Y13"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D14" sqref="D14"/>
+    <sheetView tabSelected="1" topLeftCell="M1" workbookViewId="0">
+      <selection activeCell="Q19" sqref="Q19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -805,985 +841,994 @@
     <col min="26" max="16384" width="11.42578125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:25" s="6" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E1" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="F1" s="6" t="s">
         <v>45</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="G1" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="H1" s="6" t="s">
         <v>46</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="I1" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="J1" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="K1" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="L1" s="6" t="s">
         <v>53</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="M1" s="6" t="s">
         <v>35</v>
       </c>
-      <c r="N1" s="1" t="s">
+      <c r="N1" s="6" t="s">
         <v>36</v>
       </c>
-      <c r="O1" s="1" t="s">
+      <c r="O1" s="6" t="s">
         <v>37</v>
       </c>
-      <c r="P1" s="1" t="s">
+      <c r="P1" s="6" t="s">
         <v>47</v>
       </c>
-      <c r="Q1" s="1" t="s">
+      <c r="Q1" s="6" t="s">
         <v>48</v>
       </c>
-      <c r="R1" s="1" t="s">
+      <c r="R1" s="6" t="s">
         <v>49</v>
       </c>
-      <c r="S1" s="1" t="s">
+      <c r="S1" s="6" t="s">
         <v>50</v>
       </c>
-      <c r="T1" s="1" t="s">
+      <c r="T1" s="6" t="s">
         <v>38</v>
       </c>
-      <c r="U1" s="1" t="s">
+      <c r="U1" s="6" t="s">
         <v>39</v>
       </c>
-      <c r="V1" s="1" t="s">
+      <c r="V1" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="W1" s="1" t="s">
+      <c r="W1" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="X1" s="1" t="s">
+      <c r="X1" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="Y1" s="1" t="s">
+      <c r="Y1" s="6" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="2" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A2" s="1" t="s">
+      <c r="A2" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="B2" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="C2" s="1" t="s">
+      <c r="B2" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="C2" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="D2" s="2" t="s">
+      <c r="D2" s="5" t="s">
         <v>74</v>
       </c>
-      <c r="E2" s="1" t="s">
+      <c r="E2" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="F2" s="1" t="s">
+      <c r="F2" s="4" t="s">
         <v>58</v>
       </c>
-      <c r="G2" s="1" t="s">
+      <c r="G2" s="4" t="s">
         <v>60</v>
       </c>
-      <c r="H2" s="1" t="s">
+      <c r="H2" s="4" t="s">
         <v>59</v>
       </c>
-      <c r="I2" s="1" t="s">
+      <c r="I2" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="J2" s="1">
+      <c r="J2" s="4">
         <v>9</v>
       </c>
-      <c r="K2" s="1">
+      <c r="K2" s="7">
         <v>40</v>
       </c>
-      <c r="L2" s="1">
+      <c r="L2" s="3">
         <v>120</v>
       </c>
-      <c r="M2" s="1" t="s">
+      <c r="M2" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="N2" s="1" t="s">
+      <c r="N2" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="O2" s="1" t="s">
+      <c r="O2" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="P2" s="1" t="s">
+      <c r="P2" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="Q2" s="1" t="s">
+      <c r="Q2" s="4" t="s">
         <v>51</v>
       </c>
-      <c r="R2" s="1" t="s">
+      <c r="R2" s="3" t="s">
         <v>52</v>
       </c>
-      <c r="S2" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="T2" s="1" t="s">
+      <c r="S2" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="T2" s="4" t="s">
         <v>43</v>
       </c>
-      <c r="V2" s="1" t="s">
+      <c r="U2" s="4"/>
+      <c r="V2" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="W2" s="1" t="s">
+      <c r="W2" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="X2" s="1">
+      <c r="X2" s="3">
         <v>4</v>
       </c>
-      <c r="Y2" s="1" t="s">
+      <c r="Y2" s="3" t="s">
         <v>34</v>
       </c>
     </row>
     <row r="3" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A3" s="1" t="s">
+      <c r="A3" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="B3" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="C3" s="1" t="s">
+      <c r="B3" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="C3" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="D3" s="2" t="s">
+      <c r="D3" s="5" t="s">
         <v>73</v>
       </c>
-      <c r="E3" s="1" t="s">
+      <c r="E3" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="F3" s="1" t="s">
+      <c r="F3" s="4" t="s">
         <v>58</v>
       </c>
-      <c r="G3" s="1" t="s">
+      <c r="G3" s="4" t="s">
         <v>60</v>
       </c>
-      <c r="H3" s="1" t="s">
+      <c r="H3" s="4" t="s">
         <v>59</v>
       </c>
-      <c r="I3" s="1" t="s">
+      <c r="I3" s="4" t="s">
         <v>54</v>
       </c>
-      <c r="J3" s="1">
+      <c r="J3" s="4">
         <v>9</v>
       </c>
-      <c r="K3" s="1">
+      <c r="K3" s="7">
         <v>40</v>
       </c>
-      <c r="L3" s="1">
+      <c r="L3" s="3">
         <v>120</v>
       </c>
-      <c r="M3" s="1" t="s">
+      <c r="M3" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="N3" s="1" t="s">
+      <c r="N3" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="O3" s="1" t="s">
+      <c r="O3" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="P3" s="1" t="s">
+      <c r="P3" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="Q3" s="1" t="s">
+      <c r="Q3" s="4" t="s">
         <v>51</v>
       </c>
-      <c r="R3" s="1" t="s">
+      <c r="R3" s="3" t="s">
         <v>52</v>
       </c>
-      <c r="S3" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="T3" s="1" t="s">
+      <c r="S3" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="T3" s="4" t="s">
         <v>43</v>
       </c>
-      <c r="V3" s="1" t="s">
+      <c r="U3" s="4"/>
+      <c r="V3" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="W3" s="1" t="s">
+      <c r="W3" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="X3" s="1">
+      <c r="X3" s="3">
         <v>4</v>
       </c>
-      <c r="Y3" s="1" t="s">
+      <c r="Y3" s="3" t="s">
         <v>34</v>
       </c>
     </row>
     <row r="4" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A4" s="1" t="s">
+      <c r="A4" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="B4" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="C4" s="1" t="s">
+      <c r="B4" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="C4" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="D4" s="2" t="s">
+      <c r="D4" s="5" t="s">
         <v>75</v>
       </c>
-      <c r="E4" s="1" t="s">
+      <c r="E4" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="F4" s="1" t="s">
+      <c r="F4" s="4" t="s">
         <v>58</v>
       </c>
-      <c r="G4" s="1" t="s">
+      <c r="G4" s="4" t="s">
         <v>60</v>
       </c>
-      <c r="H4" s="1" t="s">
+      <c r="H4" s="4" t="s">
         <v>59</v>
       </c>
-      <c r="I4" s="1" t="s">
+      <c r="I4" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="J4" s="1">
+      <c r="J4" s="4">
         <v>9</v>
       </c>
-      <c r="K4" s="1">
+      <c r="K4" s="7">
         <v>37</v>
       </c>
-      <c r="L4" s="1">
+      <c r="L4" s="3">
         <v>120</v>
       </c>
-      <c r="M4" s="1" t="s">
+      <c r="M4" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="N4" s="1" t="s">
+      <c r="N4" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="O4" s="1" t="s">
+      <c r="O4" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="P4" s="1" t="s">
+      <c r="P4" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="Q4" s="1" t="s">
+      <c r="Q4" s="4" t="s">
         <v>51</v>
       </c>
-      <c r="R4" s="1" t="s">
+      <c r="R4" s="3" t="s">
         <v>52</v>
       </c>
-      <c r="S4" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="T4" s="1" t="s">
+      <c r="S4" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="T4" s="4" t="s">
         <v>43</v>
       </c>
-      <c r="U4" s="1" t="s">
+      <c r="U4" s="4" t="s">
         <v>56</v>
       </c>
-      <c r="V4" s="1" t="s">
+      <c r="V4" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="W4" s="1" t="s">
+      <c r="W4" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="X4" s="1">
+      <c r="X4" s="3">
         <v>4</v>
       </c>
-      <c r="Y4" s="1" t="s">
+      <c r="Y4" s="3" t="s">
         <v>34</v>
       </c>
     </row>
     <row r="5" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A5" s="1" t="s">
+      <c r="A5" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="B5" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="C5" s="1" t="s">
+      <c r="B5" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="C5" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="D5" s="2" t="s">
+      <c r="D5" s="5" t="s">
         <v>76</v>
       </c>
-      <c r="E5" s="1" t="s">
+      <c r="E5" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="F5" s="1" t="s">
+      <c r="F5" s="4" t="s">
         <v>58</v>
       </c>
-      <c r="G5" s="1" t="s">
+      <c r="G5" s="4" t="s">
         <v>60</v>
       </c>
-      <c r="H5" s="1" t="s">
+      <c r="H5" s="4" t="s">
         <v>59</v>
       </c>
-      <c r="I5" s="1" t="s">
+      <c r="I5" s="4" t="s">
         <v>54</v>
       </c>
-      <c r="J5" s="1">
+      <c r="J5" s="4">
         <v>9</v>
       </c>
-      <c r="K5" s="1">
+      <c r="K5" s="7">
         <v>37</v>
       </c>
-      <c r="L5" s="1">
+      <c r="L5" s="3">
         <v>120</v>
       </c>
-      <c r="M5" s="1" t="s">
+      <c r="M5" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="N5" s="1" t="s">
+      <c r="N5" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="O5" s="1" t="s">
+      <c r="O5" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="P5" s="1" t="s">
+      <c r="P5" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="Q5" s="1" t="s">
+      <c r="Q5" s="4" t="s">
         <v>51</v>
       </c>
-      <c r="R5" s="1" t="s">
+      <c r="R5" s="3" t="s">
         <v>52</v>
       </c>
-      <c r="S5" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="T5" s="1" t="s">
+      <c r="S5" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="T5" s="4" t="s">
         <v>43</v>
       </c>
-      <c r="U5" s="1" t="s">
+      <c r="U5" s="4" t="s">
         <v>56</v>
       </c>
-      <c r="V5" s="1" t="s">
+      <c r="V5" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="W5" s="1" t="s">
+      <c r="W5" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="X5" s="1">
+      <c r="X5" s="3">
         <v>4</v>
       </c>
-      <c r="Y5" s="1" t="s">
+      <c r="Y5" s="3" t="s">
         <v>34</v>
       </c>
     </row>
     <row r="6" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A6" s="1" t="s">
+      <c r="A6" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="B6" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="C6" s="1" t="s">
+      <c r="B6" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="C6" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="D6" s="2" t="s">
+      <c r="D6" s="5" t="s">
         <v>77</v>
       </c>
-      <c r="E6" s="1" t="s">
+      <c r="E6" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="F6" s="1" t="s">
+      <c r="F6" s="4" t="s">
         <v>58</v>
       </c>
-      <c r="G6" s="1" t="s">
+      <c r="G6" s="4" t="s">
         <v>60</v>
       </c>
-      <c r="H6" s="1" t="s">
+      <c r="H6" s="4" t="s">
         <v>59</v>
       </c>
-      <c r="I6" s="1" t="s">
+      <c r="I6" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="J6" s="1">
+      <c r="J6" s="4">
         <v>9</v>
       </c>
-      <c r="K6" s="1">
+      <c r="K6" s="7">
         <v>70</v>
       </c>
-      <c r="L6" s="1">
+      <c r="L6" s="3">
         <v>120</v>
       </c>
-      <c r="M6" s="1" t="s">
+      <c r="M6" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="N6" s="1" t="s">
+      <c r="N6" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="O6" s="1" t="s">
+      <c r="O6" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="P6" s="1" t="s">
+      <c r="P6" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="Q6" s="1" t="s">
+      <c r="Q6" s="4" t="s">
         <v>51</v>
       </c>
-      <c r="R6" s="1" t="s">
+      <c r="R6" s="3" t="s">
         <v>52</v>
       </c>
-      <c r="S6" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="T6" s="1" t="s">
+      <c r="S6" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="T6" s="4" t="s">
         <v>43</v>
       </c>
-      <c r="V6" s="1" t="s">
+      <c r="U6" s="4"/>
+      <c r="V6" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="W6" s="1" t="s">
+      <c r="W6" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="X6" s="1">
+      <c r="X6" s="3">
         <v>4</v>
       </c>
-      <c r="Y6" s="1" t="s">
+      <c r="Y6" s="3" t="s">
         <v>34</v>
       </c>
     </row>
     <row r="7" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A7" s="1" t="s">
+      <c r="A7" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="B7" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="C7" s="1" t="s">
+      <c r="B7" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="C7" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="D7" s="2" t="s">
+      <c r="D7" s="5" t="s">
         <v>78</v>
       </c>
-      <c r="E7" s="1" t="s">
+      <c r="E7" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="F7" s="1" t="s">
+      <c r="F7" s="4" t="s">
         <v>58</v>
       </c>
-      <c r="G7" s="1" t="s">
+      <c r="G7" s="4" t="s">
         <v>60</v>
       </c>
-      <c r="H7" s="1" t="s">
+      <c r="H7" s="4" t="s">
         <v>59</v>
       </c>
-      <c r="I7" s="1" t="s">
+      <c r="I7" s="4" t="s">
         <v>54</v>
       </c>
-      <c r="J7" s="1">
+      <c r="J7" s="4">
         <v>9</v>
       </c>
-      <c r="K7" s="1">
+      <c r="K7" s="7">
         <v>70</v>
       </c>
-      <c r="L7" s="1">
+      <c r="L7" s="3">
         <v>120</v>
       </c>
-      <c r="M7" s="1" t="s">
+      <c r="M7" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="N7" s="1" t="s">
+      <c r="N7" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="O7" s="1" t="s">
+      <c r="O7" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="P7" s="1" t="s">
+      <c r="P7" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="Q7" s="1" t="s">
+      <c r="Q7" s="4" t="s">
         <v>51</v>
       </c>
-      <c r="R7" s="1" t="s">
+      <c r="R7" s="3" t="s">
         <v>52</v>
       </c>
-      <c r="S7" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="T7" s="1" t="s">
+      <c r="S7" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="T7" s="4" t="s">
         <v>43</v>
       </c>
-      <c r="V7" s="1" t="s">
+      <c r="U7" s="4"/>
+      <c r="V7" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="W7" s="1" t="s">
+      <c r="W7" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="X7" s="1">
+      <c r="X7" s="3">
         <v>4</v>
       </c>
-      <c r="Y7" s="1" t="s">
+      <c r="Y7" s="3" t="s">
         <v>34</v>
       </c>
     </row>
     <row r="8" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A8" s="1" t="s">
+      <c r="A8" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="B8" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="C8" s="1" t="s">
+      <c r="B8" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="C8" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="D8" s="2" t="s">
+      <c r="D8" s="5" t="s">
         <v>79</v>
       </c>
-      <c r="E8" s="1" t="s">
+      <c r="E8" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="F8" s="1" t="s">
+      <c r="F8" s="4" t="s">
         <v>58</v>
       </c>
-      <c r="G8" s="1" t="s">
+      <c r="G8" s="4" t="s">
         <v>60</v>
       </c>
-      <c r="H8" s="1" t="s">
+      <c r="H8" s="4" t="s">
         <v>59</v>
       </c>
-      <c r="I8" s="1" t="s">
+      <c r="I8" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="J8" s="1">
+      <c r="J8" s="4">
         <v>9</v>
       </c>
-      <c r="K8" s="1">
+      <c r="K8" s="7">
         <v>40</v>
       </c>
-      <c r="L8" s="1">
+      <c r="L8" s="3">
         <v>120</v>
       </c>
-      <c r="M8" s="1" t="s">
+      <c r="M8" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="N8" s="1" t="s">
+      <c r="N8" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="O8" s="1" t="s">
+      <c r="O8" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="P8" s="1" t="s">
+      <c r="P8" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="Q8" s="1" t="s">
+      <c r="Q8" s="4" t="s">
         <v>51</v>
       </c>
-      <c r="R8" s="1" t="s">
+      <c r="R8" s="3" t="s">
         <v>52</v>
       </c>
-      <c r="S8" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="T8" s="1" t="s">
+      <c r="S8" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="T8" s="4" t="s">
         <v>43</v>
       </c>
-      <c r="V8" s="1" t="s">
+      <c r="U8" s="4"/>
+      <c r="V8" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="W8" s="1" t="s">
+      <c r="W8" s="3" t="s">
         <v>55</v>
       </c>
-      <c r="X8" s="1">
+      <c r="X8" s="3">
         <v>4</v>
       </c>
-      <c r="Y8" s="1" t="s">
+      <c r="Y8" s="3" t="s">
         <v>34</v>
       </c>
     </row>
     <row r="9" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A9" s="1" t="s">
+      <c r="A9" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="B9" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="C9" s="1" t="s">
+      <c r="B9" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="C9" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="D9" s="2" t="s">
+      <c r="D9" s="5" t="s">
         <v>80</v>
       </c>
-      <c r="E9" s="1" t="s">
+      <c r="E9" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="F9" s="1" t="s">
+      <c r="F9" s="4" t="s">
         <v>58</v>
       </c>
-      <c r="G9" s="1" t="s">
+      <c r="G9" s="4" t="s">
         <v>60</v>
       </c>
-      <c r="H9" s="1" t="s">
+      <c r="H9" s="4" t="s">
         <v>59</v>
       </c>
-      <c r="I9" s="1" t="s">
+      <c r="I9" s="4" t="s">
         <v>54</v>
       </c>
-      <c r="J9" s="1">
+      <c r="J9" s="4">
         <v>9</v>
       </c>
-      <c r="K9" s="1">
+      <c r="K9" s="7">
         <v>40</v>
       </c>
-      <c r="L9" s="1">
+      <c r="L9" s="3">
         <v>120</v>
       </c>
-      <c r="M9" s="1" t="s">
+      <c r="M9" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="N9" s="1" t="s">
+      <c r="N9" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="O9" s="1" t="s">
+      <c r="O9" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="P9" s="1" t="s">
+      <c r="P9" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="Q9" s="1" t="s">
+      <c r="Q9" s="4" t="s">
         <v>51</v>
       </c>
-      <c r="R9" s="1" t="s">
+      <c r="R9" s="3" t="s">
         <v>52</v>
       </c>
-      <c r="S9" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="T9" s="1" t="s">
+      <c r="S9" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="T9" s="4" t="s">
         <v>43</v>
       </c>
-      <c r="V9" s="1" t="s">
+      <c r="U9" s="4"/>
+      <c r="V9" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="W9" s="1" t="s">
+      <c r="W9" s="3" t="s">
         <v>55</v>
       </c>
-      <c r="X9" s="1">
+      <c r="X9" s="3">
         <v>4</v>
       </c>
-      <c r="Y9" s="1" t="s">
+      <c r="Y9" s="3" t="s">
         <v>34</v>
       </c>
     </row>
     <row r="10" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A10" s="1" t="s">
+      <c r="A10" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="B10" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="C10" s="1" t="s">
+      <c r="B10" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="C10" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="D10" s="2" t="s">
+      <c r="D10" s="5" t="s">
         <v>81</v>
       </c>
-      <c r="E10" s="1" t="s">
+      <c r="E10" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="F10" s="1" t="s">
+      <c r="F10" s="4" t="s">
         <v>58</v>
       </c>
-      <c r="G10" s="1" t="s">
+      <c r="G10" s="4" t="s">
         <v>60</v>
       </c>
-      <c r="H10" s="1" t="s">
+      <c r="H10" s="4" t="s">
         <v>59</v>
       </c>
-      <c r="I10" s="1" t="s">
+      <c r="I10" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="J10" s="1">
+      <c r="J10" s="4">
         <v>9</v>
       </c>
-      <c r="K10" s="1">
+      <c r="K10" s="7">
         <v>37</v>
       </c>
-      <c r="L10" s="1">
+      <c r="L10" s="3">
         <v>120</v>
       </c>
-      <c r="M10" s="1" t="s">
+      <c r="M10" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="N10" s="1" t="s">
+      <c r="N10" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="O10" s="1" t="s">
+      <c r="O10" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="P10" s="1" t="s">
+      <c r="P10" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="Q10" s="1" t="s">
+      <c r="Q10" s="4" t="s">
         <v>51</v>
       </c>
-      <c r="R10" s="1" t="s">
+      <c r="R10" s="3" t="s">
         <v>52</v>
       </c>
-      <c r="S10" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="T10" s="1" t="s">
+      <c r="S10" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="T10" s="4" t="s">
         <v>43</v>
       </c>
-      <c r="U10" s="1" t="s">
+      <c r="U10" s="4" t="s">
         <v>56</v>
       </c>
-      <c r="V10" s="1" t="s">
+      <c r="V10" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="W10" s="1" t="s">
+      <c r="W10" s="3" t="s">
         <v>55</v>
       </c>
-      <c r="X10" s="1">
+      <c r="X10" s="3">
         <v>4</v>
       </c>
-      <c r="Y10" s="1" t="s">
+      <c r="Y10" s="3" t="s">
         <v>34</v>
       </c>
     </row>
     <row r="11" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A11" s="1" t="s">
+      <c r="A11" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="B11" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="C11" s="1" t="s">
+      <c r="B11" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="C11" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="D11" s="2" t="s">
+      <c r="D11" s="5" t="s">
         <v>82</v>
       </c>
-      <c r="E11" s="1" t="s">
+      <c r="E11" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="F11" s="1" t="s">
+      <c r="F11" s="4" t="s">
         <v>58</v>
       </c>
-      <c r="G11" s="1" t="s">
+      <c r="G11" s="4" t="s">
         <v>60</v>
       </c>
-      <c r="H11" s="1" t="s">
+      <c r="H11" s="4" t="s">
         <v>59</v>
       </c>
-      <c r="I11" s="1" t="s">
+      <c r="I11" s="4" t="s">
         <v>54</v>
       </c>
-      <c r="J11" s="1">
+      <c r="J11" s="4">
         <v>9</v>
       </c>
-      <c r="K11" s="1">
+      <c r="K11" s="7">
         <v>37</v>
       </c>
-      <c r="L11" s="1">
+      <c r="L11" s="3">
         <v>120</v>
       </c>
-      <c r="M11" s="1" t="s">
+      <c r="M11" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="N11" s="1" t="s">
+      <c r="N11" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="O11" s="1" t="s">
+      <c r="O11" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="P11" s="1" t="s">
+      <c r="P11" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="Q11" s="1" t="s">
+      <c r="Q11" s="4" t="s">
         <v>51</v>
       </c>
-      <c r="R11" s="1" t="s">
+      <c r="R11" s="3" t="s">
         <v>52</v>
       </c>
-      <c r="S11" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="T11" s="1" t="s">
+      <c r="S11" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="T11" s="4" t="s">
         <v>43</v>
       </c>
-      <c r="U11" s="1" t="s">
+      <c r="U11" s="4" t="s">
         <v>56</v>
       </c>
-      <c r="V11" s="1" t="s">
+      <c r="V11" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="W11" s="1" t="s">
+      <c r="W11" s="3" t="s">
         <v>55</v>
       </c>
-      <c r="X11" s="1">
+      <c r="X11" s="3">
         <v>4</v>
       </c>
-      <c r="Y11" s="1" t="s">
+      <c r="Y11" s="3" t="s">
         <v>34</v>
       </c>
     </row>
     <row r="12" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A12" s="1" t="s">
+      <c r="A12" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="B12" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="C12" s="1" t="s">
+      <c r="B12" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="C12" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="D12" s="2" t="s">
+      <c r="D12" s="5" t="s">
         <v>83</v>
       </c>
-      <c r="E12" s="1" t="s">
+      <c r="E12" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="F12" s="1" t="s">
+      <c r="F12" s="4" t="s">
         <v>58</v>
       </c>
-      <c r="G12" s="1" t="s">
+      <c r="G12" s="4" t="s">
         <v>60</v>
       </c>
-      <c r="H12" s="1" t="s">
+      <c r="H12" s="4" t="s">
         <v>59</v>
       </c>
-      <c r="I12" s="1" t="s">
+      <c r="I12" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="J12" s="1">
+      <c r="J12" s="4">
         <v>9</v>
       </c>
-      <c r="K12" s="1">
+      <c r="K12" s="7">
         <v>70</v>
       </c>
-      <c r="L12" s="1">
+      <c r="L12" s="3">
         <v>120</v>
       </c>
-      <c r="M12" s="1" t="s">
+      <c r="M12" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="N12" s="1" t="s">
+      <c r="N12" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="O12" s="1" t="s">
+      <c r="O12" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="P12" s="1" t="s">
+      <c r="P12" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="Q12" s="1" t="s">
+      <c r="Q12" s="4" t="s">
         <v>51</v>
       </c>
-      <c r="R12" s="1" t="s">
+      <c r="R12" s="3" t="s">
         <v>52</v>
       </c>
-      <c r="S12" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="T12" s="1" t="s">
+      <c r="S12" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="T12" s="4" t="s">
         <v>43</v>
       </c>
-      <c r="V12" s="1" t="s">
+      <c r="U12" s="4"/>
+      <c r="V12" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="W12" s="1" t="s">
+      <c r="W12" s="3" t="s">
         <v>55</v>
       </c>
-      <c r="X12" s="1">
+      <c r="X12" s="3">
         <v>4</v>
       </c>
-      <c r="Y12" s="1" t="s">
+      <c r="Y12" s="3" t="s">
         <v>34</v>
       </c>
     </row>
     <row r="13" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A13" s="1" t="s">
+      <c r="A13" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="B13" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="C13" s="1" t="s">
+      <c r="B13" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="C13" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="D13" s="2" t="s">
+      <c r="D13" s="5" t="s">
         <v>84</v>
       </c>
-      <c r="E13" s="1" t="s">
+      <c r="E13" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="F13" s="1" t="s">
+      <c r="F13" s="4" t="s">
         <v>58</v>
       </c>
-      <c r="G13" s="1" t="s">
+      <c r="G13" s="4" t="s">
         <v>60</v>
       </c>
-      <c r="H13" s="1" t="s">
+      <c r="H13" s="4" t="s">
         <v>59</v>
       </c>
-      <c r="I13" s="1" t="s">
+      <c r="I13" s="4" t="s">
         <v>54</v>
       </c>
-      <c r="J13" s="1">
+      <c r="J13" s="4">
         <v>9</v>
       </c>
-      <c r="K13" s="1">
+      <c r="K13" s="7">
         <v>70</v>
       </c>
-      <c r="L13" s="1">
+      <c r="L13" s="3">
         <v>120</v>
       </c>
-      <c r="M13" s="1" t="s">
+      <c r="M13" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="N13" s="1" t="s">
+      <c r="N13" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="O13" s="1" t="s">
+      <c r="O13" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="P13" s="1" t="s">
+      <c r="P13" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="Q13" s="1" t="s">
+      <c r="Q13" s="4" t="s">
         <v>51</v>
       </c>
-      <c r="R13" s="1" t="s">
+      <c r="R13" s="3" t="s">
         <v>52</v>
       </c>
-      <c r="S13" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="T13" s="1" t="s">
+      <c r="S13" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="T13" s="4" t="s">
         <v>43</v>
       </c>
-      <c r="V13" s="1" t="s">
+      <c r="U13" s="4"/>
+      <c r="V13" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="W13" s="1" t="s">
+      <c r="W13" s="3" t="s">
         <v>55</v>
       </c>
-      <c r="X13" s="1">
+      <c r="X13" s="3">
         <v>4</v>
       </c>
-      <c r="Y13" s="1" t="s">
+      <c r="Y13" s="3" t="s">
         <v>34</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -1791,8 +1836,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Z5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1827,402 +1872,402 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E1" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="F1" s="6" t="s">
         <v>45</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="G1" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="H1" s="6" t="s">
         <v>46</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="I1" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="J1" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="K1" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="L1" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="M1" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="N1" s="1" t="s">
+      <c r="N1" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="O1" s="1" t="s">
+      <c r="O1" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="P1" s="1" t="s">
+      <c r="P1" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="Q1" s="1" t="s">
+      <c r="Q1" s="6" t="s">
         <v>47</v>
       </c>
-      <c r="R1" s="1" t="s">
+      <c r="R1" s="6" t="s">
         <v>48</v>
       </c>
-      <c r="S1" s="1" t="s">
+      <c r="S1" s="6" t="s">
         <v>49</v>
       </c>
-      <c r="T1" s="1" t="s">
+      <c r="T1" s="6" t="s">
         <v>50</v>
       </c>
-      <c r="U1" s="1" t="s">
+      <c r="U1" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="V1" s="1" t="s">
+      <c r="V1" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="W1" s="1" t="s">
+      <c r="W1" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="X1" s="1" t="s">
+      <c r="X1" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="Y1" s="1" t="s">
+      <c r="Y1" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="Z1" s="1" t="s">
+      <c r="Z1" s="6" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="2" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A2" s="1" t="s">
+      <c r="A2" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="B2" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="C2" s="1" t="s">
+      <c r="B2" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="C2" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="D2" s="2" t="s">
+      <c r="D2" s="5" t="s">
         <v>69</v>
       </c>
-      <c r="E2" s="1" t="s">
+      <c r="E2" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="F2" s="1" t="s">
+      <c r="F2" s="4" t="s">
         <v>58</v>
       </c>
-      <c r="G2" s="1" t="s">
+      <c r="G2" s="4" t="s">
         <v>60</v>
       </c>
-      <c r="H2" s="1" t="s">
+      <c r="H2" s="4" t="s">
         <v>59</v>
       </c>
-      <c r="I2" s="1" t="s">
+      <c r="I2" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="J2" s="1">
+      <c r="J2" s="4">
         <v>9</v>
       </c>
-      <c r="K2" s="1">
+      <c r="K2" s="3">
         <v>300</v>
       </c>
-      <c r="L2" s="1" t="s">
+      <c r="L2" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="M2" s="1">
+      <c r="M2" s="3">
         <v>170</v>
       </c>
-      <c r="N2" s="1">
+      <c r="N2" s="3">
         <v>300</v>
       </c>
-      <c r="O2" s="1" t="s">
+      <c r="O2" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="P2" s="1" t="s">
+      <c r="P2" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="Q2" s="1" t="s">
+      <c r="Q2" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="R2" s="1" t="s">
+      <c r="R2" s="4" t="s">
         <v>51</v>
       </c>
-      <c r="S2" s="1" t="s">
+      <c r="S2" s="3" t="s">
         <v>52</v>
       </c>
-      <c r="T2" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="U2" s="1" t="s">
+      <c r="T2" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="U2" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="V2" s="1">
+      <c r="V2" s="4">
         <v>112</v>
       </c>
-      <c r="W2" s="1" t="s">
+      <c r="W2" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="X2" s="1" t="s">
+      <c r="X2" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="Y2" s="1">
+      <c r="Y2" s="3">
         <v>4</v>
       </c>
-      <c r="Z2" s="1" t="s">
+      <c r="Z2" s="3" t="s">
         <v>34</v>
       </c>
     </row>
     <row r="3" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A3" s="1" t="s">
+      <c r="A3" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="B3" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="C3" s="1" t="s">
+      <c r="B3" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="C3" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="D3" s="2" t="s">
+      <c r="D3" s="5" t="s">
         <v>70</v>
       </c>
-      <c r="E3" s="1" t="s">
+      <c r="E3" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="F3" s="1" t="s">
+      <c r="F3" s="4" t="s">
         <v>58</v>
       </c>
-      <c r="G3" s="1" t="s">
+      <c r="G3" s="4" t="s">
         <v>60</v>
       </c>
-      <c r="H3" s="1" t="s">
+      <c r="H3" s="4" t="s">
         <v>59</v>
       </c>
-      <c r="I3" s="1" t="s">
+      <c r="I3" s="4" t="s">
         <v>54</v>
       </c>
-      <c r="J3" s="1">
+      <c r="J3" s="4">
         <v>9</v>
       </c>
-      <c r="K3" s="1">
+      <c r="K3" s="3">
         <v>300</v>
       </c>
-      <c r="L3" s="1" t="s">
+      <c r="L3" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="M3" s="1">
+      <c r="M3" s="3">
         <v>170</v>
       </c>
-      <c r="N3" s="1">
+      <c r="N3" s="3">
         <v>300</v>
       </c>
-      <c r="O3" s="1" t="s">
+      <c r="O3" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="P3" s="1" t="s">
+      <c r="P3" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="Q3" s="1" t="s">
+      <c r="Q3" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="R3" s="1" t="s">
+      <c r="R3" s="4" t="s">
         <v>51</v>
       </c>
-      <c r="S3" s="1" t="s">
+      <c r="S3" s="3" t="s">
         <v>52</v>
       </c>
-      <c r="T3" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="U3" s="1" t="s">
+      <c r="T3" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="U3" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="V3" s="1">
+      <c r="V3" s="4">
         <v>112</v>
       </c>
-      <c r="W3" s="1" t="s">
+      <c r="W3" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="X3" s="1" t="s">
+      <c r="X3" s="3" t="s">
         <v>55</v>
       </c>
-      <c r="Y3" s="1">
+      <c r="Y3" s="3">
         <v>4</v>
       </c>
-      <c r="Z3" s="1" t="s">
+      <c r="Z3" s="3" t="s">
         <v>34</v>
       </c>
     </row>
     <row r="4" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A4" s="1" t="s">
+      <c r="A4" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="B4" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="C4" s="1" t="s">
+      <c r="B4" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="C4" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="D4" s="2" t="s">
+      <c r="D4" s="5" t="s">
         <v>71</v>
       </c>
-      <c r="E4" s="1" t="s">
+      <c r="E4" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="F4" s="1" t="s">
+      <c r="F4" s="4" t="s">
         <v>58</v>
       </c>
-      <c r="G4" s="1" t="s">
+      <c r="G4" s="4" t="s">
         <v>60</v>
       </c>
-      <c r="H4" s="1" t="s">
+      <c r="H4" s="4" t="s">
         <v>59</v>
       </c>
-      <c r="I4" s="1" t="s">
+      <c r="I4" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="J4" s="1">
+      <c r="J4" s="4">
         <v>9</v>
       </c>
-      <c r="K4" s="1">
+      <c r="K4" s="3">
         <v>300</v>
       </c>
-      <c r="L4" s="1" t="s">
+      <c r="L4" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="M4" s="1">
+      <c r="M4" s="3">
         <v>170</v>
       </c>
-      <c r="N4" s="1">
+      <c r="N4" s="3">
         <v>300</v>
       </c>
-      <c r="O4" s="1" t="s">
+      <c r="O4" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="P4" s="1" t="s">
+      <c r="P4" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="Q4" s="1" t="s">
+      <c r="Q4" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="R4" s="1" t="s">
+      <c r="R4" s="4" t="s">
         <v>51</v>
       </c>
-      <c r="S4" s="1" t="s">
+      <c r="S4" s="3" t="s">
         <v>52</v>
       </c>
-      <c r="T4" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="U4" s="1" t="s">
+      <c r="T4" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="U4" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="V4" s="1">
+      <c r="V4" s="4">
         <v>112</v>
       </c>
-      <c r="W4" s="1" t="s">
+      <c r="W4" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="X4" s="1" t="s">
+      <c r="X4" s="3" t="s">
         <v>55</v>
       </c>
-      <c r="Y4" s="1">
+      <c r="Y4" s="3">
         <v>4</v>
       </c>
-      <c r="Z4" s="1" t="s">
+      <c r="Z4" s="3" t="s">
         <v>34</v>
       </c>
     </row>
     <row r="5" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A5" s="1" t="s">
+      <c r="A5" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="B5" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="C5" s="1" t="s">
+      <c r="B5" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="C5" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="D5" s="2" t="s">
+      <c r="D5" s="5" t="s">
         <v>72</v>
       </c>
-      <c r="E5" s="1" t="s">
+      <c r="E5" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="F5" s="1" t="s">
+      <c r="F5" s="4" t="s">
         <v>58</v>
       </c>
-      <c r="G5" s="1" t="s">
+      <c r="G5" s="4" t="s">
         <v>60</v>
       </c>
-      <c r="H5" s="1" t="s">
+      <c r="H5" s="4" t="s">
         <v>59</v>
       </c>
-      <c r="I5" s="1" t="s">
+      <c r="I5" s="4" t="s">
         <v>54</v>
       </c>
-      <c r="J5" s="1">
+      <c r="J5" s="4">
         <v>9</v>
       </c>
-      <c r="K5" s="1">
+      <c r="K5" s="3">
         <v>300</v>
       </c>
-      <c r="L5" s="1" t="s">
+      <c r="L5" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="M5" s="1">
+      <c r="M5" s="3">
         <v>170</v>
       </c>
-      <c r="N5" s="1">
+      <c r="N5" s="3">
         <v>300</v>
       </c>
-      <c r="O5" s="1" t="s">
+      <c r="O5" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="P5" s="1" t="s">
+      <c r="P5" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="Q5" s="1" t="s">
+      <c r="Q5" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="R5" s="1" t="s">
+      <c r="R5" s="4" t="s">
         <v>51</v>
       </c>
-      <c r="S5" s="1" t="s">
+      <c r="S5" s="3" t="s">
         <v>52</v>
       </c>
-      <c r="T5" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="U5" s="1" t="s">
+      <c r="T5" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="U5" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="V5" s="1">
+      <c r="V5" s="4">
         <v>112</v>
       </c>
-      <c r="W5" s="1" t="s">
+      <c r="W5" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="X5" s="1" t="s">
+      <c r="X5" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="Y5" s="1">
+      <c r="Y5" s="3">
         <v>4</v>
       </c>
-      <c r="Z5" s="1" t="s">
+      <c r="Z5" s="3" t="s">
         <v>34</v>
       </c>
     </row>
@@ -2236,7 +2281,7 @@
   <dimension ref="A1:W3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+      <selection activeCell="A2" sqref="A2:XFD2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2268,215 +2313,215 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="D1" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E1" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="F1" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="G1" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="H1" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="I1" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="J1" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="K1" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="L1" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="M1" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="N1" s="1" t="s">
+      <c r="N1" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="O1" s="1" t="s">
+      <c r="O1" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="P1" s="1" t="s">
+      <c r="P1" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="Q1" s="1" t="s">
+      <c r="Q1" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="R1" s="1" t="s">
+      <c r="R1" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="S1" s="1" t="s">
+      <c r="S1" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="T1" s="1" t="s">
+      <c r="T1" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="U1" s="1" t="s">
+      <c r="U1" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="V1" s="1" t="s">
+      <c r="V1" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="W1" s="1" t="s">
+      <c r="W1" s="6" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="2" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A2" s="1" t="s">
+      <c r="A2" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="B2" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="C2" s="1" t="s">
+      <c r="B2" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="C2" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="D2" s="2" t="s">
+      <c r="D2" s="5" t="s">
         <v>67</v>
       </c>
-      <c r="E2" s="1" t="s">
+      <c r="E2" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="F2" s="1" t="s">
+      <c r="F2" s="4" t="s">
         <v>58</v>
       </c>
-      <c r="G2" s="1" t="s">
+      <c r="G2" s="4" t="s">
         <v>60</v>
       </c>
-      <c r="H2" s="1" t="s">
+      <c r="H2" s="4" t="s">
         <v>59</v>
       </c>
-      <c r="I2" s="1" t="s">
+      <c r="I2" s="4" t="s">
         <v>57</v>
       </c>
-      <c r="J2" s="1">
+      <c r="J2" s="4">
         <v>9</v>
       </c>
-      <c r="K2" s="1">
+      <c r="K2" s="3">
         <v>300</v>
       </c>
-      <c r="L2" s="1" t="s">
+      <c r="L2" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="M2" s="1">
+      <c r="M2" s="3">
         <v>170</v>
       </c>
-      <c r="N2" s="1">
+      <c r="N2" s="3">
         <v>300</v>
       </c>
-      <c r="O2" s="1" t="s">
+      <c r="O2" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="P2" s="1" t="s">
+      <c r="P2" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="Q2" s="1" t="s">
+      <c r="Q2" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="R2" s="1">
+      <c r="R2" s="4">
         <v>123</v>
       </c>
-      <c r="S2" s="1" t="s">
+      <c r="S2" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="T2" s="1" t="s">
+      <c r="T2" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="U2" s="1" t="s">
+      <c r="U2" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="V2" s="1">
+      <c r="V2" s="4">
         <v>4</v>
       </c>
-      <c r="W2" s="1" t="s">
+      <c r="W2" s="4" t="s">
         <v>34</v>
       </c>
     </row>
     <row r="3" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A3" s="1" t="s">
+      <c r="A3" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="B3" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="C3" s="1" t="s">
+      <c r="B3" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="C3" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="D3" s="2" t="s">
+      <c r="D3" s="5" t="s">
         <v>68</v>
       </c>
-      <c r="E3" s="1" t="s">
+      <c r="E3" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="F3" s="1" t="s">
+      <c r="F3" s="4" t="s">
         <v>58</v>
       </c>
-      <c r="G3" s="1" t="s">
+      <c r="G3" s="4" t="s">
         <v>60</v>
       </c>
-      <c r="H3" s="1" t="s">
+      <c r="H3" s="4" t="s">
         <v>59</v>
       </c>
-      <c r="I3" s="1" t="s">
+      <c r="I3" s="4" t="s">
         <v>57</v>
       </c>
-      <c r="J3" s="1">
+      <c r="J3" s="4">
         <v>9</v>
       </c>
-      <c r="K3" s="1">
+      <c r="K3" s="3">
         <v>300</v>
       </c>
-      <c r="L3" s="1" t="s">
+      <c r="L3" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="M3" s="1">
+      <c r="M3" s="3">
         <v>170</v>
       </c>
-      <c r="N3" s="1">
+      <c r="N3" s="3">
         <v>300</v>
       </c>
-      <c r="O3" s="1" t="s">
+      <c r="O3" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="P3" s="1" t="s">
+      <c r="P3" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="Q3" s="1" t="s">
+      <c r="Q3" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="R3" s="1">
+      <c r="R3" s="4">
         <v>123</v>
       </c>
-      <c r="S3" s="1" t="s">
+      <c r="S3" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="T3" s="1" t="s">
+      <c r="T3" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="U3" s="1" t="s">
+      <c r="U3" s="4" t="s">
         <v>55</v>
       </c>
-      <c r="V3" s="1">
+      <c r="V3" s="4">
         <v>4</v>
       </c>
-      <c r="W3" s="1" t="s">
+      <c r="W3" s="4" t="s">
         <v>34</v>
       </c>
     </row>
@@ -2490,7 +2535,7 @@
   <dimension ref="A1:V7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2521,466 +2566,470 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="D1" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E1" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="F1" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="G1" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="H1" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="I1" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="J1" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="K1" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="L1" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="M1" s="6" t="s">
         <v>35</v>
       </c>
-      <c r="N1" s="1" t="s">
+      <c r="N1" s="6" t="s">
         <v>36</v>
       </c>
-      <c r="O1" s="1" t="s">
+      <c r="O1" s="6" t="s">
         <v>37</v>
       </c>
-      <c r="P1" s="1" t="s">
+      <c r="P1" s="6" t="s">
         <v>38</v>
       </c>
-      <c r="Q1" s="1" t="s">
+      <c r="Q1" s="6" t="s">
         <v>39</v>
       </c>
-      <c r="R1" s="1" t="s">
+      <c r="R1" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="S1" s="1" t="s">
+      <c r="S1" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="T1" s="1" t="s">
+      <c r="T1" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="U1" s="1" t="s">
+      <c r="U1" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="V1" s="1" t="s">
+      <c r="V1" s="6" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="2" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A2" s="1" t="s">
+      <c r="A2" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="B2" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="C2" s="1" t="s">
+      <c r="B2" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="C2" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="D2" s="2" t="s">
+      <c r="D2" s="5" t="s">
         <v>61</v>
       </c>
-      <c r="E2" s="1" t="s">
+      <c r="E2" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="F2" s="1" t="s">
+      <c r="F2" s="4" t="s">
         <v>58</v>
       </c>
-      <c r="G2" s="1" t="s">
+      <c r="G2" s="4" t="s">
         <v>60</v>
       </c>
-      <c r="H2" s="1" t="s">
+      <c r="H2" s="4" t="s">
         <v>59</v>
       </c>
-      <c r="I2" s="1" t="s">
+      <c r="I2" s="4" t="s">
         <v>57</v>
       </c>
-      <c r="J2" s="1">
+      <c r="J2" s="4">
         <v>12</v>
       </c>
-      <c r="K2" s="1">
+      <c r="K2" s="3">
         <v>40</v>
       </c>
-      <c r="L2" s="1">
+      <c r="L2" s="3">
         <v>120</v>
       </c>
-      <c r="M2" s="1" t="s">
+      <c r="M2" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="N2" s="1" t="s">
+      <c r="N2" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="O2" s="1" t="s">
+      <c r="O2" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="P2" s="1" t="s">
+      <c r="P2" s="3" t="s">
         <v>43</v>
       </c>
-      <c r="R2" s="1" t="s">
+      <c r="Q2" s="3"/>
+      <c r="R2" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="S2" s="1" t="s">
+      <c r="S2" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="T2" s="1" t="s">
+      <c r="T2" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="U2" s="1">
+      <c r="U2" s="3">
         <v>4</v>
       </c>
-      <c r="V2" s="1" t="s">
+      <c r="V2" s="3" t="s">
         <v>34</v>
       </c>
     </row>
     <row r="3" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A3" s="1" t="s">
+      <c r="A3" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="B3" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="C3" s="1" t="s">
+      <c r="B3" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="C3" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="D3" s="2" t="s">
+      <c r="D3" s="5" t="s">
         <v>62</v>
       </c>
-      <c r="E3" s="1" t="s">
+      <c r="E3" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="F3" s="1" t="s">
+      <c r="F3" s="4" t="s">
         <v>58</v>
       </c>
-      <c r="G3" s="1" t="s">
+      <c r="G3" s="4" t="s">
         <v>60</v>
       </c>
-      <c r="H3" s="1" t="s">
+      <c r="H3" s="4" t="s">
         <v>59</v>
       </c>
-      <c r="I3" s="1" t="s">
+      <c r="I3" s="4" t="s">
         <v>57</v>
       </c>
-      <c r="J3" s="1">
+      <c r="J3" s="4">
         <v>9</v>
       </c>
-      <c r="K3" s="1">
+      <c r="K3" s="3">
         <v>37</v>
       </c>
-      <c r="L3" s="1">
+      <c r="L3" s="3">
         <v>120</v>
       </c>
-      <c r="M3" s="1" t="s">
+      <c r="M3" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="N3" s="1" t="s">
+      <c r="N3" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="O3" s="1" t="s">
+      <c r="O3" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="P3" s="1" t="s">
+      <c r="P3" s="3" t="s">
         <v>43</v>
       </c>
-      <c r="Q3" s="1" t="s">
+      <c r="Q3" s="3" t="s">
         <v>56</v>
       </c>
-      <c r="R3" s="1" t="s">
+      <c r="R3" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="S3" s="1" t="s">
+      <c r="S3" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="T3" s="1" t="s">
+      <c r="T3" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="U3" s="1">
+      <c r="U3" s="3">
         <v>4</v>
       </c>
-      <c r="V3" s="1" t="s">
+      <c r="V3" s="3" t="s">
         <v>34</v>
       </c>
     </row>
     <row r="4" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A4" s="1" t="s">
+      <c r="A4" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="B4" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="C4" s="1" t="s">
+      <c r="B4" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="C4" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="D4" s="2" t="s">
+      <c r="D4" s="5" t="s">
         <v>63</v>
       </c>
-      <c r="E4" s="1" t="s">
+      <c r="E4" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="F4" s="1" t="s">
+      <c r="F4" s="4" t="s">
         <v>58</v>
       </c>
-      <c r="G4" s="1" t="s">
+      <c r="G4" s="4" t="s">
         <v>60</v>
       </c>
-      <c r="H4" s="1" t="s">
+      <c r="H4" s="4" t="s">
         <v>59</v>
       </c>
-      <c r="I4" s="1" t="s">
+      <c r="I4" s="4" t="s">
         <v>57</v>
       </c>
-      <c r="J4" s="1">
+      <c r="J4" s="4">
         <v>9</v>
       </c>
-      <c r="K4" s="1">
+      <c r="K4" s="3">
         <v>70</v>
       </c>
-      <c r="L4" s="1">
+      <c r="L4" s="3">
         <v>47</v>
       </c>
-      <c r="M4" s="1" t="s">
+      <c r="M4" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="N4" s="1" t="s">
+      <c r="N4" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="O4" s="1" t="s">
+      <c r="O4" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="P4" s="1" t="s">
+      <c r="P4" s="3" t="s">
         <v>43</v>
       </c>
-      <c r="R4" s="1" t="s">
+      <c r="Q4" s="3"/>
+      <c r="R4" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="S4" s="1" t="s">
+      <c r="S4" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="T4" s="1" t="s">
+      <c r="T4" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="U4" s="1">
+      <c r="U4" s="3">
         <v>4</v>
       </c>
-      <c r="V4" s="1" t="s">
+      <c r="V4" s="3" t="s">
         <v>34</v>
       </c>
     </row>
     <row r="5" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A5" s="1" t="s">
+      <c r="A5" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="B5" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="C5" s="1" t="s">
+      <c r="B5" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="C5" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="D5" s="2" t="s">
+      <c r="D5" s="5" t="s">
         <v>64</v>
       </c>
-      <c r="E5" s="1" t="s">
+      <c r="E5" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="F5" s="1" t="s">
+      <c r="F5" s="4" t="s">
         <v>58</v>
       </c>
-      <c r="G5" s="1" t="s">
+      <c r="G5" s="4" t="s">
         <v>60</v>
       </c>
-      <c r="H5" s="1" t="s">
+      <c r="H5" s="4" t="s">
         <v>59</v>
       </c>
-      <c r="I5" s="1" t="s">
+      <c r="I5" s="4" t="s">
         <v>57</v>
       </c>
-      <c r="J5" s="1">
+      <c r="J5" s="4">
         <v>9</v>
       </c>
-      <c r="K5" s="1">
+      <c r="K5" s="3">
         <v>40</v>
       </c>
-      <c r="L5" s="1">
+      <c r="L5" s="3">
         <v>120</v>
       </c>
-      <c r="M5" s="1" t="s">
+      <c r="M5" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="N5" s="1" t="s">
+      <c r="N5" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="O5" s="1" t="s">
+      <c r="O5" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="P5" s="1" t="s">
+      <c r="P5" s="3" t="s">
         <v>43</v>
       </c>
-      <c r="R5" s="1" t="s">
+      <c r="Q5" s="3"/>
+      <c r="R5" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="S5" s="1" t="s">
+      <c r="S5" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="T5" s="1" t="s">
+      <c r="T5" s="3" t="s">
         <v>55</v>
       </c>
-      <c r="U5" s="1">
+      <c r="U5" s="3">
         <v>4</v>
       </c>
-      <c r="V5" s="1" t="s">
+      <c r="V5" s="3" t="s">
         <v>34</v>
       </c>
     </row>
     <row r="6" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A6" s="1" t="s">
+      <c r="A6" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="B6" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="C6" s="1" t="s">
+      <c r="B6" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="C6" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="D6" s="2" t="s">
+      <c r="D6" s="5" t="s">
         <v>65</v>
       </c>
-      <c r="E6" s="1" t="s">
+      <c r="E6" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="F6" s="1" t="s">
+      <c r="F6" s="4" t="s">
         <v>58</v>
       </c>
-      <c r="G6" s="1" t="s">
+      <c r="G6" s="4" t="s">
         <v>60</v>
       </c>
-      <c r="H6" s="1" t="s">
+      <c r="H6" s="4" t="s">
         <v>59</v>
       </c>
-      <c r="I6" s="1" t="s">
+      <c r="I6" s="4" t="s">
         <v>57</v>
       </c>
-      <c r="J6" s="1">
+      <c r="J6" s="4">
         <v>10</v>
       </c>
-      <c r="K6" s="1">
+      <c r="K6" s="3">
         <v>37</v>
       </c>
-      <c r="L6" s="1">
+      <c r="L6" s="3">
         <v>120</v>
       </c>
-      <c r="M6" s="1" t="s">
+      <c r="M6" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="N6" s="1" t="s">
+      <c r="N6" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="O6" s="1" t="s">
+      <c r="O6" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="P6" s="1" t="s">
+      <c r="P6" s="3" t="s">
         <v>43</v>
       </c>
-      <c r="Q6" s="1" t="s">
+      <c r="Q6" s="3" t="s">
         <v>56</v>
       </c>
-      <c r="R6" s="1" t="s">
+      <c r="R6" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="S6" s="1" t="s">
+      <c r="S6" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="T6" s="1" t="s">
+      <c r="T6" s="3" t="s">
         <v>55</v>
       </c>
-      <c r="U6" s="1">
+      <c r="U6" s="3">
         <v>4</v>
       </c>
-      <c r="V6" s="1" t="s">
+      <c r="V6" s="3" t="s">
         <v>34</v>
       </c>
     </row>
     <row r="7" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A7" s="1" t="s">
+      <c r="A7" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="B7" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="C7" s="1" t="s">
+      <c r="B7" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="C7" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="D7" s="2" t="s">
+      <c r="D7" s="5" t="s">
         <v>66</v>
       </c>
-      <c r="E7" s="1" t="s">
+      <c r="E7" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="F7" s="1" t="s">
+      <c r="F7" s="4" t="s">
         <v>58</v>
       </c>
-      <c r="G7" s="1" t="s">
+      <c r="G7" s="4" t="s">
         <v>60</v>
       </c>
-      <c r="H7" s="1" t="s">
+      <c r="H7" s="4" t="s">
         <v>59</v>
       </c>
-      <c r="I7" s="1" t="s">
+      <c r="I7" s="4" t="s">
         <v>57</v>
       </c>
-      <c r="J7" s="1">
+      <c r="J7" s="4">
         <v>9</v>
       </c>
-      <c r="K7" s="1">
+      <c r="K7" s="3">
         <v>70</v>
       </c>
-      <c r="L7" s="1">
+      <c r="L7" s="3">
         <v>120</v>
       </c>
-      <c r="M7" s="1" t="s">
+      <c r="M7" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="N7" s="1" t="s">
+      <c r="N7" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="O7" s="1" t="s">
+      <c r="O7" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="P7" s="1" t="s">
+      <c r="P7" s="3" t="s">
         <v>43</v>
       </c>
-      <c r="R7" s="1" t="s">
+      <c r="Q7" s="3"/>
+      <c r="R7" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="S7" s="1" t="s">
+      <c r="S7" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="T7" s="1" t="s">
+      <c r="T7" s="3" t="s">
         <v>55</v>
       </c>
-      <c r="U7" s="1">
+      <c r="U7" s="3">
         <v>4</v>
       </c>
-      <c r="V7" s="1" t="s">
+      <c r="V7" s="3" t="s">
         <v>34</v>
       </c>
     </row>

</xml_diff>